<commit_message>
Module 5: add functionality for getting and adding professor details
</commit_message>
<xml_diff>
--- a/professor.xlsx
+++ b/professor.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8090a3a5aa513dda/Desktop/DATA 200/Assignments/Data200-Lab1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{2CE47529-7E7A-4445-8A40-F8D8552A0B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43770E48-5DAF-40D2-8B54-96E9F4F4067E}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{2CE47529-7E7A-4445-8A40-F8D8552A0B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C197575F-C577-4746-91FB-80D47BE43F21}"/>
   <bookViews>
-    <workbookView xWindow="42030" yWindow="3375" windowWidth="19200" windowHeight="10275" xr2:uid="{4182EF1D-540C-4EBE-9D4D-D528A0DBD6F4}"/>
+    <workbookView xWindow="38685" yWindow="2280" windowWidth="21600" windowHeight="11175" xr2:uid="{4182EF1D-540C-4EBE-9D4D-D528A0DBD6F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>professor_id</t>
   </si>
@@ -48,7 +48,19 @@
     <t>John Smith</t>
   </si>
   <si>
-    <t>Data200</t>
+    <t>DATA201</t>
+  </si>
+  <si>
+    <t>DATA200</t>
+  </si>
+  <si>
+    <t>Visiting Lecturer</t>
+  </si>
+  <si>
+    <t>Ken Douglas</t>
+  </si>
+  <si>
+    <t>douglas@myschool.edu</t>
   </si>
 </sst>
 </file>
@@ -431,15 +443,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECF7EA4-6BE8-4785-B3AB-D0A2FC52BD1D}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.54296875" customWidth="1"/>
     <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1796875" customWidth="1"/>
@@ -470,12 +482,27 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{25B144FA-ACE2-403D-86CB-DBA7A1DCF334}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{7458C52D-F373-4819-B5B7-487825D926F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>